<commit_message>
add update bug popup function from view bug table
</commit_message>
<xml_diff>
--- a/bug_reports.xlsx
+++ b/bug_reports.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,7 +481,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Closed</t>
+          <t>In Progress</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-08-02 12:08:03</t>
+          <t>2023-08-02 16:31:58</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Open</t>
+          <t>Closed</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-08-02 14:11:05</t>
+          <t>2023-08-02 16:57:38</t>
         </is>
       </c>
     </row>
@@ -626,12 +626,12 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>fgfgfg</t>
+          <t>fgfg clossed</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Open</t>
+          <t>Closed</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-08-02 14:47:32</t>
+          <t>2023-08-02 16:56:51</t>
         </is>
       </c>
     </row>
@@ -656,22 +656,82 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>printer is working</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2023-08-02 15:04:47</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2023-08-02 16:58:24</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>fan not working</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>fan not working</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2023-08-02 17:09:57</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2023-08-02 17:10:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>printer is not working</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Closed</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>2023-08-02 15:04:47</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>2023-08-02 15:17:37</t>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>printer is not working</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2023-08-02 17:10:04</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2023-08-02 17:10:27</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
auto refresh on table implemented
</commit_message>
<xml_diff>
--- a/bug_reports.xlsx
+++ b/bug_reports.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,12 +476,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dfsfa dafdfdaf fdfad</t>
+          <t>not fixed</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>Open</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-08-02 16:31:58</t>
+          <t>2023-08-03 14:48:21</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Closed</t>
+          <t>Open</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-08-02 16:56:51</t>
+          <t>2023-08-03 16:16:08</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>Closed</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -671,7 +671,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-08-02 16:58:24</t>
+          <t>2023-08-03 13:03:56</t>
         </is>
       </c>
     </row>
@@ -732,6 +732,156 @@
       <c r="F10" t="inlineStr">
         <is>
           <t>2023-08-02 17:10:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>good bye</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>good bye</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2023-08-03 13:06:27</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2023-08-03 13:06:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>auto refresh</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>auto refresh</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2023-08-03 14:18:12</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2023-08-03 14:56:56</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>dddd</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>dddd</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2023-08-03 14:57:06</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2023-08-03 16:06:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>godjflkdaj</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>godjflkdaj</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2023-08-03 15:58:29</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2023-08-03 16:05:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>321</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>weqweq</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>weqweq</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2023-08-03 16:15:50</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2023-08-03 16:16:20</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Css changes in main page
</commit_message>
<xml_diff>
--- a/bug_reports.xlsx
+++ b/bug_reports.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,12 +476,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>not fixed</t>
+          <t>fixed</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Open</t>
+          <t>Closed</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -491,7 +491,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-08-03 14:48:21</t>
+          <t>2023-08-11 14:40:28</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-08-02 13:02:54</t>
+          <t>2023-08-11 15:15:13</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Open</t>
+          <t>Closed</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-08-03 16:16:08</t>
+          <t>2023-08-04 16:07:02</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>Closed</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2023-08-02 17:10:14</t>
+          <t>2023-08-04 16:06:53</t>
         </is>
       </c>
     </row>
@@ -871,17 +871,137 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>2023-08-03 16:15:50</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2023-08-04 08:24:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>567</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>fdsfsdfs</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>fdsfsdfs</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>Closed</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2023-08-03 16:15:50</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2023-08-03 16:16:20</t>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>2023-08-04 08:24:46</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2023-08-04 16:07:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>3242</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>sewrewr</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>sewrewr</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>2023-08-04 08:25:01</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2023-08-04 08:29:45</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>314</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>erewrw</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>erewrw</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Closed</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>2023-08-04 08:25:11</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2023-08-04 16:07:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>999</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>good work as bug</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>good work as bug is working</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>In Progress</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>2023-08-11 15:47:32</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2023-08-11 15:48:45</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Delete function implemented in but data table
</commit_message>
<xml_diff>
--- a/bug_reports.xlsx
+++ b/bug_reports.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,196 +467,196 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dfsfa</t>
+          <t>auto refresh</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>fixed</t>
+          <t>auto refresh</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Closed</t>
+          <t>In Progress</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2023-08-02 12:07:10</t>
+          <t>2023-08-03 14:18:12</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-08-11 14:40:28</t>
+          <t>2023-08-03 14:56:56</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>34</v>
+        <v>100</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>dfad</t>
+          <t>godjflkdaj</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dfad working</t>
+          <t>godjflkdaj</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>Closed</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2023-08-02 12:07:51</t>
+          <t>2023-08-03 15:58:29</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2023-08-11 15:15:13</t>
+          <t>2023-08-03 16:05:52</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>12</v>
+        <v>321</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>good country</t>
+          <t>weqweq</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>good country</t>
+          <t>weqweq</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Closed</t>
+          <t>In Progress</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2023-08-02 14:11:05</t>
+          <t>2023-08-03 16:15:50</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2023-08-02 16:57:38</t>
+          <t>2023-08-04 08:24:28</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>23</v>
+        <v>567</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>fan not working</t>
+          <t>fdsfsdfs</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fan not working</t>
+          <t>fdsfsdfs</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>Closed</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2023-08-02 14:15:54</t>
+          <t>2023-08-04 08:24:46</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2023-08-02 14:16:07</t>
+          <t>2023-08-04 16:07:19</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>56</v>
+        <v>314</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>afdf</t>
+          <t>erewrw</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>afdf</t>
+          <t>erewrw</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>In Progress</t>
+          <t>Closed</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2023-08-02 14:45:09</t>
+          <t>2023-08-04 08:25:11</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2023-08-02 14:47:18</t>
+          <t>2023-08-04 16:07:29</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>111</v>
+        <v>999</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>fgfgfg</t>
+          <t>good work as bug</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>fgfg clossed</t>
+          <t>good work as bug is working</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Closed</t>
+          <t>In Progress</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>2023-08-02 14:47:32</t>
+          <t>2023-08-11 15:47:32</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2023-08-04 16:07:02</t>
+          <t>2023-08-11 15:48:45</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>5555</v>
+        <v>1000</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>printer is not working</t>
+          <t>good morning</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>printer is working</t>
+          <t>good morning working</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -666,342 +666,12 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>2023-08-02 15:04:47</t>
+          <t>2023-08-12 10:00:55</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2023-08-03 13:03:56</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>fan not working</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>fan not working</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Closed</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>2023-08-02 17:09:57</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>2023-08-04 16:06:53</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>printer is not working</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>printer is not working</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>In Progress</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>2023-08-02 17:10:04</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2023-08-02 17:10:27</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>good bye</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>good bye</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Closed</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>2023-08-03 13:06:27</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>2023-08-03 13:06:50</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>auto refresh</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>auto refresh</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>In Progress</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2023-08-03 14:18:12</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>2023-08-03 14:56:56</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="1" t="n">
-        <v>22</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>dddd</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>dddd</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Closed</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>2023-08-03 14:57:06</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>2023-08-03 16:06:03</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>godjflkdaj</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>godjflkdaj</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Closed</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>2023-08-03 15:58:29</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>2023-08-03 16:05:52</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1" t="n">
-        <v>321</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>weqweq</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>weqweq</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>In Progress</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>2023-08-03 16:15:50</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>2023-08-04 08:24:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="n">
-        <v>567</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>fdsfsdfs</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>fdsfsdfs</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Closed</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>2023-08-04 08:24:46</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>2023-08-04 16:07:19</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="n">
-        <v>3242</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>sewrewr</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>sewrewr</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Closed</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>2023-08-04 08:25:01</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>2023-08-04 08:29:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="n">
-        <v>314</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>erewrw</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>erewrw</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Closed</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>2023-08-04 08:25:11</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>2023-08-04 16:07:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="1" t="n">
-        <v>999</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>good work as bug</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>good work as bug is working</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>In Progress</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>2023-08-11 15:47:32</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>2023-08-11 15:48:45</t>
+          <t>2023-08-14 10:37:06</t>
         </is>
       </c>
     </row>

</xml_diff>